<commit_message>
regressao aplicada na malha pt1
</commit_message>
<xml_diff>
--- a/apa/gdf2.xlsx
+++ b/apa/gdf2.xlsx
@@ -600,7 +600,7 @@
         <v>-42924.77015087473</v>
       </c>
       <c r="L3" t="n">
-        <v>170193.796239063</v>
+        <v>170193.7962390623</v>
       </c>
     </row>
     <row r="4">
@@ -759,7 +759,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>-38417.07184248177</v>
+        <v>-38417.07184248176</v>
       </c>
       <c r="L6" t="n">
         <v>166057.8584131754</v>
@@ -1029,7 +1029,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>-79666.82331478485</v>
+        <v>-79666.82331478484</v>
       </c>
       <c r="L11" t="n">
         <v>-110615.535824162</v>
@@ -1083,7 +1083,7 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>-82644.30700047665</v>
+        <v>-82644.30700047668</v>
       </c>
       <c r="L12" t="n">
         <v>-115839.1324620537</v>
@@ -1137,10 +1137,10 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>-85332.85319380002</v>
+        <v>-85332.85319379999</v>
       </c>
       <c r="L13" t="n">
-        <v>-103298.2947739012</v>
+        <v>-103298.2947739005</v>
       </c>
     </row>
     <row r="14">
@@ -1947,10 +1947,10 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>-13646.36265228279</v>
+        <v>-13646.36265228278</v>
       </c>
       <c r="L28" t="n">
-        <v>197834.0127053966</v>
+        <v>197834.0127053973</v>
       </c>
     </row>
     <row r="29">
@@ -2004,7 +2004,7 @@
         <v>28635.95884533177</v>
       </c>
       <c r="L29" t="n">
-        <v>189170.9787543955</v>
+        <v>189170.9787543962</v>
       </c>
     </row>
     <row r="30">
@@ -2271,7 +2271,7 @@
         </is>
       </c>
       <c r="K34" t="n">
-        <v>-45621.89032152404</v>
+        <v>-45621.89032152403</v>
       </c>
       <c r="L34" t="n">
         <v>102590.1969691089</v>
@@ -2649,10 +2649,10 @@
         </is>
       </c>
       <c r="K41" t="n">
-        <v>-65679.59472312924</v>
+        <v>-65679.59472312922</v>
       </c>
       <c r="L41" t="n">
-        <v>-126634.1711313672</v>
+        <v>-126634.1711313679</v>
       </c>
     </row>
     <row r="42">
@@ -2811,7 +2811,7 @@
         </is>
       </c>
       <c r="K44" t="n">
-        <v>-64535.07110579082</v>
+        <v>-64535.07110579083</v>
       </c>
       <c r="L44" t="n">
         <v>-125942.7294961648</v>
@@ -3351,10 +3351,10 @@
         </is>
       </c>
       <c r="K54" t="n">
-        <v>-96115.9370233228</v>
+        <v>-96115.93702332278</v>
       </c>
       <c r="L54" t="n">
-        <v>-42518.17937972415</v>
+        <v>-42518.17937972344</v>
       </c>
     </row>
     <row r="55">
@@ -3408,7 +3408,7 @@
         <v>-48640.1828791037</v>
       </c>
       <c r="L55" t="n">
-        <v>-114310.1729534447</v>
+        <v>-114310.172953444</v>
       </c>
     </row>
     <row r="56">
@@ -3462,7 +3462,7 @@
         <v>-49218.58775434551</v>
       </c>
       <c r="L56" t="n">
-        <v>182292.3852031552</v>
+        <v>182292.3852031559</v>
       </c>
     </row>
     <row r="57">
@@ -3999,10 +3999,10 @@
         </is>
       </c>
       <c r="K66" t="n">
-        <v>-81372.6836666842</v>
+        <v>-81372.68366668421</v>
       </c>
       <c r="L66" t="n">
-        <v>-111421.3437174443</v>
+        <v>-111421.343717445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>